<commit_message>
Basic web server ready at port 3000
</commit_message>
<xml_diff>
--- a/misc_files/BuildSteps.xlsx
+++ b/misc_files/BuildSteps.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
   <si>
     <t>NodeJS - MongoDB, Mongoose, Express, Gulp, Backbone, React, Semantic</t>
   </si>
@@ -33,18 +33,6 @@
     <t>make directory</t>
   </si>
   <si>
-    <t>npm init</t>
-  </si>
-  <si>
-    <t>copy ssh path</t>
-  </si>
-  <si>
-    <t>creates package.json dependency list in root</t>
-  </si>
-  <si>
-    <t>create git repo</t>
-  </si>
-  <si>
     <t>npm install express --save</t>
   </si>
   <si>
@@ -63,16 +51,10 @@
     <t>location</t>
   </si>
   <si>
-    <t>github/terminal</t>
-  </si>
-  <si>
     <t>github</t>
   </si>
   <si>
     <t>browser</t>
-  </si>
-  <si>
-    <t>node app.js</t>
   </si>
   <si>
     <t>server.js</t>
@@ -116,6 +98,53 @@
   </si>
   <si>
     <t>commit first clean revision of project</t>
+  </si>
+  <si>
+    <t>copy ssh path from github</t>
+  </si>
+  <si>
+    <t>create github repo</t>
+  </si>
+  <si>
+    <t>git remote add (your choosen name of remote, ex. jedi) (github path)</t>
+  </si>
+  <si>
+    <t>git pull (remote name) master</t>
+  </si>
+  <si>
+    <t>master is the default branch for a new github repo</t>
+  </si>
+  <si>
+    <t>git push (remote name) master</t>
+  </si>
+  <si>
+    <t>push local directory to github repo</t>
+  </si>
+  <si>
+    <t>node server.js</t>
+  </si>
+  <si>
+    <t>touch server.start.js</t>
+  </si>
+  <si>
+    <t>set up http server environment on host server (taken from express-generate bin/www)</t>
+  </si>
+  <si>
+    <t>package.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "scripts": {
+    "start": "node ./server.start.js"
+  },</t>
+  </si>
+  <si>
+    <t>nodemon will use this to run the start file before launching server.js, the backend of the app</t>
+  </si>
+  <si>
+    <t>script.sh</t>
+  </si>
+  <si>
+    <t>default node packages for all projects - before deciding on specific project dependencies</t>
   </si>
 </sst>
 </file>
@@ -177,14 +206,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -198,12 +237,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -533,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -554,116 +606,103 @@
     </row>
     <row r="2" spans="1:3" ht="27" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="27" customHeight="1">
-      <c r="A3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="20" customHeight="1"/>
     <row r="4" spans="1:3" ht="27" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="27" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="27" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>2</v>
+        <v>19</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="27" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="27" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="27" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="27" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="27" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="27" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="27" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>21</v>
+        <v>7</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="27" customHeight="1">
@@ -671,18 +710,21 @@
         <v>11</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="185" customHeight="1">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="27" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>19</v>
+        <v>7</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="27" customHeight="1">
@@ -690,18 +732,92 @@
         <v>11</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" ht="27" customHeight="1"/>
-    <row r="18" ht="27" customHeight="1"/>
-    <row r="19" ht="27" customHeight="1"/>
-    <row r="20" ht="27" customHeight="1"/>
-    <row r="21" ht="27" customHeight="1"/>
-    <row r="22" ht="27" customHeight="1"/>
+    </row>
+    <row r="17" spans="1:3" ht="27" customHeight="1">
+      <c r="A17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="185" customHeight="1">
+      <c r="A18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="27" customHeight="1">
+      <c r="A19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="27" customHeight="1">
+      <c r="A20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="27" customHeight="1">
+      <c r="B21" s="3"/>
+    </row>
+    <row r="22" spans="1:3" ht="27" customHeight="1">
+      <c r="B22" s="3"/>
+    </row>
+    <row r="23" spans="1:3" ht="27" customHeight="1">
+      <c r="B23" s="3"/>
+    </row>
+    <row r="24" spans="1:3" ht="27" customHeight="1">
+      <c r="B24" s="3"/>
+    </row>
+    <row r="25" spans="1:3" ht="27" customHeight="1">
+      <c r="B25" s="3"/>
+    </row>
+    <row r="26" spans="1:3" ht="27" customHeight="1">
+      <c r="A26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="95" customHeight="1">
+      <c r="A27" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="27" customHeight="1"/>
+    <row r="29" spans="1:3" ht="27" customHeight="1"/>
+    <row r="30" spans="1:3" ht="27" customHeight="1"/>
+    <row r="31" spans="1:3" ht="27" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>